<commit_message>
Finished, added some conclusions and thoughts
</commit_message>
<xml_diff>
--- a/LAB/Disease_detection/hyperparameter_tuning_results_dataset1.xlsx
+++ b/LAB/Disease_detection/hyperparameter_tuning_results_dataset1.xlsx
@@ -468,11 +468,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'C': 0.01, 'solver': 'newton-cg'}</t>
+          <t>{'C': 1.0, 'solver': 'liblinear'}</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.6990788469093643</v>
+        <v>0.7029875880182564</v>
       </c>
     </row>
     <row r="3">
@@ -488,11 +488,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'criterion': 'entropy', 'max_depth': 5}</t>
+          <t>{'criterion': 'entropy', 'max_depth': 8}</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.6953853275998387</v>
+        <v>0.6990582330233022</v>
       </c>
     </row>
     <row r="4">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.6989929662326182</v>
+        <v>0.7032578647725752</v>
       </c>
     </row>
     <row r="5">
@@ -528,11 +528,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'learning_rate': 0.1, 'max_depth': 5, 'n_estimators': 100}</t>
+          <t>{'learning_rate': 0.1, 'max_depth': 3, 'n_estimators': 200}</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.7006035765069739</v>
+        <v>0.7047132008094686</v>
       </c>
     </row>
     <row r="6">
@@ -548,11 +548,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'C': 0.1, 'solver': 'newton-cg'}</t>
+          <t>{'C': 100.0, 'solver': 'newton-cg'}</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.6989929685383253</v>
+        <v>0.7029875880182564</v>
       </c>
     </row>
     <row r="7">
@@ -568,11 +568,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'criterion': 'entropy', 'max_depth': 5}</t>
+          <t>{'criterion': 'entropy', 'max_depth': 8}</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.6953853275998387</v>
+        <v>0.698954282919352</v>
       </c>
     </row>
     <row r="8">
@@ -588,11 +588,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'max_depth': 10, 'min_samples_split': 10, 'n_estimators': 200}</t>
+          <t>{'max_depth': 10, 'min_samples_split': 2, 'n_estimators': 200}</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.6994654448385947</v>
+        <v>0.7031954839034577</v>
       </c>
     </row>
     <row r="9">
@@ -608,11 +608,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'learning_rate': 0.1, 'max_depth': 5, 'n_estimators': 100}</t>
+          <t>{'learning_rate': 0.1, 'max_depth': 3, 'n_estimators': 200}</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.7005176727731555</v>
+        <v>0.7047339886689091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>